<commit_message>
Mensaje descriptivo de tus cambios
</commit_message>
<xml_diff>
--- a/Asignaciones/upl/uploads/datos_exceldatos1_1714747072.xlsx
+++ b/Asignaciones/upl/uploads/datos_exceldatos1_1714747072.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juams\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9711C732-0BB4-46CA-B238-04C72C9DD51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABAFD14-4969-437E-9B15-6C48884004A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4257,14 +4257,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B579C1C-7897-4286-8D69-47046EA099D2}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AH552"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B75" sqref="B75"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4406,7 +4405,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="119">
         <v>2067390</v>
       </c>
@@ -4450,7 +4449,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="124">
         <v>2068318</v>
       </c>
@@ -4530,7 +4529,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="124">
         <v>2068319</v>
       </c>
@@ -4580,7 +4579,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="124">
         <v>2068323</v>
       </c>
@@ -4630,7 +4629,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="124">
         <v>2104624</v>
       </c>
@@ -4680,7 +4679,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="124">
         <v>2104625</v>
       </c>
@@ -4730,7 +4729,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="124">
         <v>2104626</v>
       </c>
@@ -4780,7 +4779,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="124">
         <v>2104627</v>
       </c>
@@ -4830,7 +4829,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="124">
         <v>2104628</v>
       </c>
@@ -4880,7 +4879,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="124">
         <v>2104629</v>
       </c>
@@ -4930,7 +4929,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="124">
         <v>2104714</v>
       </c>
@@ -4980,7 +4979,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="124">
         <v>2104715</v>
       </c>
@@ -5030,7 +5029,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="124">
         <v>2104716</v>
       </c>
@@ -5080,7 +5079,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="124">
         <v>2104717</v>
       </c>
@@ -5130,7 +5129,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="124">
         <v>2104718</v>
       </c>
@@ -5180,7 +5179,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="124">
         <v>2104719</v>
       </c>
@@ -5230,7 +5229,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="124">
         <v>2104720</v>
       </c>
@@ -5280,7 +5279,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="124">
         <v>2104721</v>
       </c>
@@ -5330,7 +5329,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="124">
         <v>2104784</v>
       </c>
@@ -5380,7 +5379,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="124">
         <v>2104785</v>
       </c>
@@ -5430,7 +5429,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="124">
         <v>2104786</v>
       </c>
@@ -5480,7 +5479,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="124">
         <v>2104787</v>
       </c>
@@ -5530,7 +5529,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="124">
         <v>2104788</v>
       </c>
@@ -5580,7 +5579,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="124">
         <v>2104789</v>
       </c>
@@ -5630,7 +5629,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="124">
         <v>2104790</v>
       </c>
@@ -5680,7 +5679,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="124">
         <v>2104791</v>
       </c>
@@ -5730,7 +5729,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="124">
         <v>2104792</v>
       </c>
@@ -5780,7 +5779,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="124">
         <v>2104793</v>
       </c>
@@ -5830,7 +5829,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="124">
         <v>2104794</v>
       </c>
@@ -5880,7 +5879,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="124">
         <v>2104795</v>
       </c>
@@ -5930,7 +5929,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="124">
         <v>2104796</v>
       </c>
@@ -5980,7 +5979,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="124">
         <v>2104797</v>
       </c>
@@ -6030,7 +6029,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="124">
         <v>2104798</v>
       </c>
@@ -6080,7 +6079,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="124">
         <v>2104799</v>
       </c>
@@ -6130,7 +6129,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="124">
         <v>2104861</v>
       </c>
@@ -6180,7 +6179,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="124">
         <v>2104862</v>
       </c>
@@ -6230,7 +6229,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="124">
         <v>2104863</v>
       </c>
@@ -6280,7 +6279,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="124">
         <v>2104864</v>
       </c>
@@ -6330,7 +6329,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="124">
         <v>2104865</v>
       </c>
@@ -6380,7 +6379,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="124">
         <v>2104866</v>
       </c>
@@ -6430,7 +6429,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="124">
         <v>2104901</v>
       </c>
@@ -6480,7 +6479,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="124">
         <v>2104902</v>
       </c>
@@ -6530,7 +6529,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="124">
         <v>2120525</v>
       </c>
@@ -6580,7 +6579,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="124">
         <v>2120527</v>
       </c>
@@ -6630,7 +6629,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="185">
         <v>2141776</v>
       </c>
@@ -6685,7 +6684,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="72">
         <v>2141791</v>
       </c>
@@ -6770,7 +6769,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
         <v>2142207</v>
       </c>
@@ -6855,7 +6854,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14">
         <v>2142234</v>
       </c>
@@ -6940,7 +6939,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14">
         <v>2142237</v>
       </c>
@@ -7025,7 +7024,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
         <v>2142240</v>
       </c>
@@ -7110,7 +7109,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>2142254</v>
       </c>
@@ -7195,7 +7194,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="72">
         <v>2164554</v>
       </c>
@@ -7250,7 +7249,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
         <v>2164626</v>
       </c>
@@ -7335,7 +7334,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>2175790</v>
       </c>
@@ -7420,7 +7419,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>2175791</v>
       </c>
@@ -7505,7 +7504,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
         <v>2175792</v>
       </c>
@@ -7560,7 +7559,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10">
         <v>2175793</v>
       </c>
@@ -7615,7 +7614,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>2175794</v>
       </c>
@@ -7670,7 +7669,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
         <v>2175795</v>
       </c>
@@ -7725,7 +7724,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
         <v>2175796</v>
       </c>
@@ -7780,7 +7779,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10">
         <v>2175797</v>
       </c>
@@ -7835,7 +7834,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
         <v>2175798</v>
       </c>
@@ -7890,7 +7889,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10">
         <v>2175799</v>
       </c>
@@ -7945,7 +7944,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10">
         <v>2175800</v>
       </c>
@@ -8000,7 +7999,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
         <v>2175801</v>
       </c>
@@ -8055,7 +8054,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
         <v>2175802</v>
       </c>
@@ -8110,7 +8109,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10">
         <v>2175803</v>
       </c>
@@ -8165,7 +8164,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10">
         <v>2175804</v>
       </c>
@@ -8220,7 +8219,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10">
         <v>2175805</v>
       </c>
@@ -8275,7 +8274,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10">
         <v>2183159</v>
       </c>
@@ -8358,7 +8357,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10">
         <v>2183172</v>
       </c>
@@ -8441,7 +8440,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10">
         <v>2183174</v>
       </c>
@@ -8524,7 +8523,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10">
         <v>2205024</v>
       </c>
@@ -8779,7 +8778,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:31" s="64" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:31" s="64" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="72">
         <v>2205052</v>
       </c>
@@ -8946,7 +8945,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:31" s="31" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:31" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="57">
         <v>2205070</v>
       </c>
@@ -9002,7 +9001,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="221">
         <v>2205087</v>
       </c>
@@ -9087,7 +9086,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="10">
         <v>2206979</v>
       </c>
@@ -9426,7 +9425,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="65">
         <v>2234834</v>
       </c>
@@ -9482,7 +9481,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10">
         <v>2234847</v>
       </c>
@@ -9622,7 +9621,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="221">
         <v>2234908</v>
       </c>
@@ -9838,7 +9837,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14">
         <v>2234971</v>
       </c>
@@ -9923,7 +9922,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14">
         <v>2234974</v>
       </c>
@@ -10178,7 +10177,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="14">
         <v>2235173</v>
       </c>
@@ -10496,7 +10495,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:31" s="38" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="10">
         <v>2253486</v>
       </c>
@@ -10552,7 +10551,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="102" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="10">
         <v>2253487</v>
       </c>
@@ -10637,7 +10636,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="33">
         <v>2253488</v>
       </c>
@@ -10721,7 +10720,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="104" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="72">
         <v>2253496</v>
       </c>
@@ -10806,7 +10805,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="72">
         <v>2253497</v>
       </c>
@@ -10861,7 +10860,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="221">
         <v>2253498</v>
       </c>
@@ -10946,7 +10945,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:31" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10">
         <v>2253499</v>
       </c>
@@ -11001,7 +11000,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="10">
         <v>2253500</v>
       </c>
@@ -11086,7 +11085,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="14">
         <v>2253501</v>
       </c>
@@ -11481,7 +11480,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="10">
         <v>2257839</v>
       </c>
@@ -11536,7 +11535,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="10">
         <v>2262833</v>
       </c>
@@ -12686,7 +12685,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="133" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="14">
         <v>2274933</v>
       </c>
@@ -12762,7 +12761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="134" spans="1:31" s="31" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:31" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="10">
         <v>2274935</v>
       </c>
@@ -12818,7 +12817,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="135" spans="1:31" s="31" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:31" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="10">
         <v>2274937</v>
       </c>
@@ -13045,7 +13044,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="138" spans="1:31" s="31" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:31" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="10">
         <v>2275952</v>
       </c>
@@ -13215,7 +13214,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="140" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="10">
         <v>2275956</v>
       </c>
@@ -13386,7 +13385,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="142" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="10">
         <v>2275981</v>
       </c>
@@ -14294,7 +14293,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="154" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="10">
         <v>2278170</v>
       </c>
@@ -14377,7 +14376,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="155" spans="1:31" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="14">
         <v>2278173</v>
       </c>
@@ -14460,7 +14459,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="156" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="14">
         <v>2278617</v>
       </c>
@@ -14545,7 +14544,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="157" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="72">
         <v>2279611</v>
       </c>
@@ -14850,7 +14849,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="161" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="14">
         <v>2280351</v>
       </c>
@@ -14935,7 +14934,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="162" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="72">
         <v>2280374</v>
       </c>
@@ -15623,7 +15622,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="172" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="221">
         <v>2315457</v>
       </c>
@@ -15878,7 +15877,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="175" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="14">
         <v>2322481</v>
       </c>
@@ -16018,7 +16017,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="177" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="14">
         <v>2322977</v>
       </c>
@@ -16268,7 +16267,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="181" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="72">
         <v>2337822</v>
       </c>
@@ -16323,7 +16322,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="182" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="14">
         <v>2337946</v>
       </c>
@@ -16631,7 +16630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="186" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="10">
         <v>2338761</v>
       </c>
@@ -16686,7 +16685,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="187" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="10">
         <v>2338762</v>
       </c>
@@ -16741,7 +16740,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="188" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="10">
         <v>2338763</v>
       </c>
@@ -16796,7 +16795,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="189" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="10">
         <v>2338764</v>
       </c>
@@ -16851,7 +16850,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="190" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="10">
         <v>2338783</v>
       </c>
@@ -16906,7 +16905,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="191" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="10">
         <v>2338784</v>
       </c>
@@ -16961,7 +16960,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="192" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="10">
         <v>2339412</v>
       </c>
@@ -17131,7 +17130,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="194" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="10">
         <v>2339417</v>
       </c>
@@ -17214,7 +17213,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="195" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="14">
         <v>2339420</v>
       </c>
@@ -17354,7 +17353,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="197" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="72">
         <v>2339428</v>
       </c>
@@ -17439,7 +17438,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="198" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="72">
         <v>2340136</v>
       </c>
@@ -17494,7 +17493,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="199" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="72">
         <v>2340137</v>
       </c>
@@ -17604,7 +17603,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="201" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="10">
         <v>2341304</v>
       </c>
@@ -17689,7 +17688,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="202" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="221">
         <v>2341307</v>
       </c>
@@ -17884,7 +17883,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="205" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="10">
         <v>2348252</v>
       </c>
@@ -17969,7 +17968,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="206" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="10">
         <v>2348315</v>
       </c>
@@ -18054,7 +18053,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="207" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="10">
         <v>2348388</v>
       </c>
@@ -18194,7 +18193,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="209" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="10">
         <v>2348493</v>
       </c>
@@ -18968,7 +18967,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="220" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="14">
         <v>2364594</v>
       </c>
@@ -19053,7 +19052,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="221" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="14">
         <v>2364616</v>
       </c>
@@ -19333,7 +19332,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="225" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="10">
         <v>2374507</v>
       </c>
@@ -19418,7 +19417,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="226" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="10">
         <v>2374566</v>
       </c>
@@ -19503,7 +19502,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="227" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="10">
         <v>2374616</v>
       </c>
@@ -19558,7 +19557,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="228" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="10">
         <v>2374657</v>
       </c>
@@ -19613,7 +19612,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="229" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="10">
         <v>2374784</v>
       </c>
@@ -19668,7 +19667,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="230" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="10">
         <v>2374793</v>
       </c>
@@ -19723,7 +19722,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="231" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="10">
         <v>2374795</v>
       </c>
@@ -19778,7 +19777,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="232" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="14">
         <v>2374805</v>
       </c>
@@ -19833,7 +19832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="233" spans="1:31" s="45" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:31" s="45" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="14">
         <v>2374814</v>
       </c>
@@ -19889,7 +19888,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="234" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="14">
         <v>2374816</v>
       </c>
@@ -19944,7 +19943,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="235" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="42">
         <v>2381189</v>
       </c>
@@ -20287,7 +20286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="239" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="14">
         <v>2381282</v>
       </c>
@@ -20374,7 +20373,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="240" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="72">
         <v>2381295</v>
       </c>
@@ -20461,7 +20460,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="241" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="221">
         <v>2381315</v>
       </c>
@@ -20633,7 +20632,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="243" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="14">
         <v>2386426</v>
       </c>
@@ -20688,7 +20687,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="244" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="14">
         <v>2387624</v>
       </c>
@@ -20743,7 +20742,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="245" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="14">
         <v>2387625</v>
       </c>
@@ -20883,7 +20882,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="247" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="10">
         <v>2394005</v>
       </c>
@@ -20968,7 +20967,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="248" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="14">
         <v>2394013</v>
       </c>
@@ -21053,7 +21052,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="249" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="10">
         <v>2394039</v>
       </c>
@@ -21108,7 +21107,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="250" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="10">
         <v>2394064</v>
       </c>
@@ -21218,7 +21217,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="252" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="14">
         <v>2395494</v>
       </c>
@@ -21308,7 +21307,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="14">
         <v>2398800</v>
       </c>
@@ -21448,7 +21447,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="255" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="14">
         <v>2404289</v>
       </c>
@@ -21533,7 +21532,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="256" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="7">
         <v>2404838</v>
       </c>
@@ -21923,7 +21922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="262" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="10">
         <v>2409545</v>
       </c>
@@ -22033,7 +22032,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="264" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="10">
         <v>2418258</v>
       </c>
@@ -22088,7 +22087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="265" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="14">
         <v>2418609</v>
       </c>
@@ -22258,7 +22257,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="267" spans="1:31" s="31" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:31" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="72">
         <v>2427268</v>
       </c>
@@ -22348,7 +22347,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="268" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="14">
         <v>2427271</v>
       </c>
@@ -22436,7 +22435,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="269" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="10">
         <v>2427295</v>
       </c>
@@ -22522,7 +22521,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="270" spans="1:31" s="31" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:31" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="14">
         <v>2427299</v>
       </c>
@@ -22722,7 +22721,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="273" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="42">
         <v>2436827</v>
       </c>
@@ -22808,7 +22807,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="274" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="14">
         <v>2437960</v>
       </c>
@@ -22969,7 +22968,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="276" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="182">
         <v>2450121</v>
       </c>
@@ -23256,7 +23255,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="280" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="72">
         <v>2450163</v>
       </c>
@@ -23316,7 +23315,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="281" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="47">
         <v>2450179</v>
       </c>
@@ -23406,7 +23405,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="282" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" s="47">
         <v>2450210</v>
       </c>
@@ -23496,7 +23495,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="283" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="221">
         <v>2450214</v>
       </c>
@@ -23584,7 +23583,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="284" spans="1:31" s="31" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:31" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="10">
         <v>2450238</v>
       </c>
@@ -23644,7 +23643,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="285" spans="1:31" s="31" customFormat="1" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:31" s="31" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="49">
         <v>2450243</v>
       </c>
@@ -23732,7 +23731,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="286" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="10">
         <v>2450246</v>
       </c>
@@ -23906,7 +23905,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="288" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="10">
         <v>2453547</v>
       </c>
@@ -23994,7 +23993,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="289" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="10">
         <v>2455172</v>
       </c>
@@ -24136,7 +24135,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="291" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="10">
         <v>2455248</v>
       </c>
@@ -24306,7 +24305,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="293" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="14">
         <v>2455886</v>
       </c>
@@ -24391,7 +24390,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="294" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="10">
         <v>2472753</v>
       </c>
@@ -24448,7 +24447,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="295" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="10">
         <v>2472754</v>
       </c>
@@ -24505,7 +24504,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="296" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="72">
         <v>2472758</v>
       </c>
@@ -24562,7 +24561,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="297" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="49">
         <v>2472767</v>
       </c>
@@ -24650,7 +24649,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="298" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="49">
         <v>2472800</v>
       </c>
@@ -24820,7 +24819,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="301" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="10">
         <v>2477532</v>
       </c>
@@ -24932,7 +24931,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="303" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="14">
         <v>2479271</v>
       </c>
@@ -25101,7 +25100,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="305" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" s="14">
         <v>2489354</v>
       </c>
@@ -25327,7 +25326,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="308" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="14">
         <v>2499966</v>
       </c>
@@ -25412,7 +25411,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="309" spans="1:31" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="14">
         <v>2500135</v>
       </c>
@@ -26108,7 +26107,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="319" spans="1:31" s="31" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:31" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A319" s="73">
         <v>2500395</v>
       </c>
@@ -26195,7 +26194,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="320" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A320" s="73">
         <v>2500402</v>
       </c>
@@ -26280,7 +26279,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="321" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" s="73">
         <v>2500419</v>
       </c>
@@ -26420,7 +26419,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="323" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" s="73">
         <v>2500424</v>
       </c>
@@ -26475,7 +26474,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="324" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A324" s="73">
         <v>2500428</v>
       </c>
@@ -26560,7 +26559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="325" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A325" s="73">
         <v>2500430</v>
       </c>
@@ -26645,7 +26644,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="326" spans="1:31" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="49">
         <v>2500436</v>
       </c>
@@ -26733,7 +26732,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="327" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A327" s="182">
         <v>2500438</v>
       </c>
@@ -26793,7 +26792,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="328" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A328" s="49">
         <v>2500477</v>
       </c>
@@ -26883,7 +26882,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="329" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A329" s="182">
         <v>2500481</v>
       </c>
@@ -26943,7 +26942,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="330" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A330" s="73">
         <v>2500591</v>
       </c>
@@ -26998,7 +26997,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="331" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A331" s="73">
         <v>2500603</v>
       </c>
@@ -27053,7 +27052,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="332" spans="1:31" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A332" s="73">
         <v>2500612</v>
       </c>
@@ -27108,7 +27107,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="333" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A333" s="73">
         <v>2500804</v>
       </c>
@@ -27193,7 +27192,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="334" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="182">
         <v>2501110</v>
       </c>
@@ -28509,7 +28508,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="352" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A352" s="73">
         <v>2539569</v>
       </c>
@@ -28704,7 +28703,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="355" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A355" s="238">
         <v>2548016</v>
       </c>
@@ -28759,7 +28758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="356" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A356" s="14">
         <v>2548674</v>
       </c>
@@ -29012,7 +29011,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="359" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A359" s="73">
         <v>2557641</v>
       </c>
@@ -29097,7 +29096,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="360" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A360" s="73">
         <v>2557685</v>
       </c>
@@ -29182,7 +29181,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="361" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A361" s="73">
         <v>2557699</v>
       </c>
@@ -29435,7 +29434,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="364" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A364" s="47">
         <v>2557924</v>
       </c>
@@ -29512,7 +29511,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="365" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A365" s="73">
         <v>2557948</v>
       </c>
@@ -29567,7 +29566,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="366" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A366" s="73">
         <v>2557985</v>
       </c>
@@ -29652,7 +29651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="367" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A367" s="73">
         <v>2558029</v>
       </c>
@@ -29735,7 +29734,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="368" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A368" s="49">
         <v>2558036</v>
       </c>
@@ -29782,7 +29781,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="369" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A369" s="49">
         <v>2558046</v>
       </c>
@@ -29827,7 +29826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="370" spans="1:31" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:31" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A370" s="49">
         <v>2558058</v>
       </c>
@@ -29876,7 +29875,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="371" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A371" s="49">
         <v>2558068</v>
       </c>
@@ -30087,7 +30086,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="374" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A374" s="10">
         <v>2559138</v>
       </c>
@@ -30263,7 +30262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="377" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A377" s="235">
         <v>2559171</v>
       </c>
@@ -30310,7 +30309,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="378" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A378" s="235">
         <v>2559172</v>
       </c>
@@ -30550,7 +30549,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="382" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A382" s="14">
         <v>2594955</v>
       </c>
@@ -30864,7 +30863,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="386" spans="1:31" s="31" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:31" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A386" s="47">
         <v>2598327</v>
       </c>
@@ -30942,7 +30941,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="387" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A387" s="235">
         <v>2601765</v>
       </c>
@@ -31074,7 +31073,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="389" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A389" s="14">
         <v>2604939</v>
       </c>
@@ -31159,7 +31158,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="390" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A390" s="47">
         <v>2605469</v>
       </c>
@@ -31236,7 +31235,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="391" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A391" s="14">
         <v>2613919</v>
       </c>
@@ -31463,7 +31462,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="394" spans="1:31" s="31" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:31" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A394" s="47">
         <v>2617847</v>
       </c>
@@ -31543,7 +31542,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="395" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A395" s="47">
         <v>2617857</v>
       </c>
@@ -31622,7 +31621,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="396" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A396" s="47">
         <v>2617865</v>
       </c>
@@ -31701,7 +31700,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="397" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A397" s="47">
         <v>2617866</v>
       </c>
@@ -31778,7 +31777,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="398" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A398" s="47">
         <v>2617943</v>
       </c>
@@ -31997,7 +31996,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="401" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A401" s="47">
         <v>2618351</v>
       </c>
@@ -32074,7 +32073,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="402" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A402" s="235">
         <v>2618378</v>
       </c>
@@ -32121,7 +32120,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="403" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A403" s="47">
         <v>2618383</v>
       </c>
@@ -32198,7 +32197,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="404" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A404" s="47">
         <v>2618384</v>
       </c>
@@ -32275,7 +32274,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="405" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A405" s="235">
         <v>2618385</v>
       </c>
@@ -32322,7 +32321,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="406" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A406" s="47">
         <v>2618843</v>
       </c>
@@ -32369,7 +32368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="407" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A407" s="47">
         <v>2619021</v>
       </c>
@@ -32418,7 +32417,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="408" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A408" s="47">
         <v>2619661</v>
       </c>
@@ -32465,7 +32464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="409" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A409" s="47">
         <v>2619696</v>
       </c>
@@ -32512,7 +32511,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="410" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A410" s="47">
         <v>2619706</v>
       </c>
@@ -32677,7 +32676,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="412" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A412" s="82">
         <v>2621926</v>
       </c>
@@ -32904,7 +32903,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="415" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A415" s="192">
         <v>2626910</v>
       </c>
@@ -32981,7 +32980,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="416" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A416" s="192">
         <v>2626911</v>
       </c>
@@ -33058,7 +33057,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="417" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A417" s="192">
         <v>2627027</v>
       </c>
@@ -33135,7 +33134,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="418" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A418" s="192">
         <v>2627028</v>
       </c>
@@ -33212,7 +33211,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="419" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A419" s="192">
         <v>2627029</v>
       </c>
@@ -33656,7 +33655,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="426" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A426" s="87">
         <v>2656975</v>
       </c>
@@ -34021,7 +34020,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="431" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A431" s="83">
         <v>2670521</v>
       </c>
@@ -34271,7 +34270,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="434" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A434" s="83">
         <v>2694768</v>
       </c>
@@ -34375,7 +34374,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="436" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A436" s="164">
         <v>2696186</v>
       </c>
@@ -34898,7 +34897,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="442" spans="1:31" ht="28.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:31" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A442" s="82">
         <v>2701306</v>
       </c>
@@ -35301,7 +35300,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="448" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A448" s="164">
         <v>2703292</v>
       </c>
@@ -35768,7 +35767,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="454" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A454" s="87">
         <v>2708500</v>
       </c>
@@ -35855,7 +35854,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="455" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A455" s="82">
         <v>2708535</v>
       </c>
@@ -36479,7 +36478,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="464" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A464" s="164">
         <v>2710823</v>
       </c>
@@ -36736,7 +36735,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="467" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A467" s="82">
         <v>2717781</v>
       </c>
@@ -36793,7 +36792,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="468" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A468" s="164">
         <v>2717788</v>
       </c>
@@ -38200,7 +38199,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="488" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A488" s="87">
         <v>2778458</v>
       </c>
@@ -38257,7 +38256,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="489" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A489" s="87">
         <v>2787115</v>
       </c>
@@ -38849,7 +38848,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="497" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A497" s="74">
         <v>2820937</v>
       </c>
@@ -38905,7 +38904,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="498" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A498" s="74">
         <v>2821004</v>
       </c>
@@ -39474,7 +39473,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="508" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A508" s="87">
         <v>2843540</v>
       </c>
@@ -39551,7 +39550,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="509" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A509" s="87">
         <v>2849294</v>
       </c>
@@ -39675,7 +39674,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="511" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A511" s="87">
         <v>2855111</v>
       </c>
@@ -39722,7 +39721,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="512" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A512" s="87">
         <v>2869410</v>
       </c>
@@ -40000,7 +39999,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="516" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A516" s="202">
         <v>2874985</v>
       </c>
@@ -40043,7 +40042,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="517" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A517" s="200">
         <v>2874986</v>
       </c>
@@ -40087,7 +40086,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="518" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A518" s="77">
         <v>2670037</v>
       </c>
@@ -40124,7 +40123,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="519" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A519" s="77">
         <v>2670050</v>
       </c>
@@ -40161,7 +40160,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="520" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A520" s="77">
         <v>2670053</v>
       </c>
@@ -40198,7 +40197,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="521" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A521" s="77">
         <v>2670475</v>
       </c>
@@ -40235,7 +40234,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="522" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A522" s="77">
         <v>2670488</v>
       </c>
@@ -40272,7 +40271,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="523" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A523" s="77">
         <v>2675725</v>
       </c>
@@ -40309,7 +40308,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="524" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A524" s="77">
         <v>2675736</v>
       </c>
@@ -40346,7 +40345,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="525" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A525" s="77">
         <v>2675737</v>
       </c>
@@ -40383,7 +40382,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="526" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A526" s="77">
         <v>2675738</v>
       </c>
@@ -40420,7 +40419,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="527" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A527" s="77">
         <v>2675897</v>
       </c>
@@ -40457,7 +40456,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="528" spans="1:31" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A528" s="77">
         <v>2682751</v>
       </c>
@@ -40494,7 +40493,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="529" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A529" s="77">
         <v>2694461</v>
       </c>
@@ -40531,7 +40530,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="530" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A530" s="77">
         <v>2694462</v>
       </c>
@@ -40568,7 +40567,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="531" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A531" s="77">
         <v>2694467</v>
       </c>
@@ -40605,7 +40604,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="532" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A532" s="77">
         <v>2694472</v>
       </c>
@@ -40642,7 +40641,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="533" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A533" s="77">
         <v>2694474</v>
       </c>
@@ -40679,7 +40678,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="534" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A534" s="77">
         <v>2694476</v>
       </c>
@@ -40716,7 +40715,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="535" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A535" s="77">
         <v>2708498</v>
       </c>
@@ -40753,7 +40752,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="536" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A536" s="77">
         <v>2708510</v>
       </c>
@@ -41197,7 +41196,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="548" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A548" s="77">
         <v>2914536</v>
       </c>
@@ -41234,7 +41233,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="549" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A549" s="77">
         <v>2931901</v>
       </c>
@@ -41271,7 +41270,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="550" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A550" s="77">
         <v>2921179</v>
       </c>
@@ -41345,7 +41344,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="552" spans="1:14" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A552" s="77">
         <v>2963885</v>
       </c>
@@ -41383,14 +41382,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE552" xr:uid="{6B579C1C-7897-4286-8D69-47046EA099D2}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="TECNICO"/>
-        <filter val="TÉCNICO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AE552" xr:uid="{6B579C1C-7897-4286-8D69-47046EA099D2}"/>
   <conditionalFormatting sqref="A1:A99 A101:A517 A553:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
@@ -58868,6 +58860,71 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="bd192ae8-048c-430e-a712-bd4d6e23679a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c84e791c-9279-4101-b0d8-1359c6bfb8a8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="bd192ae8-048c-430e-a712-bd4d6e23679a">
+      <UserInfo>
+        <DisplayName>Magda Bibiana Claros Rodriguez</DisplayName>
+        <AccountId>20</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Diana Patricia Murillo Quintero</DisplayName>
+        <AccountId>90</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Gerson Alejandro Saavedra Molano</DisplayName>
+        <AccountId>30</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Miguel Antonio Portilla Castro</DisplayName>
+        <AccountId>24</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan Evangelista Luna Luna</DisplayName>
+        <AccountId>36</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sandra Carolina Pena</DisplayName>
+        <AccountId>23</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Angela Daniela Naranjo Vanegas</DisplayName>
+        <AccountId>237</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>cuentadecobrocic</DisplayName>
+        <AccountId>293</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PENDIENTE xmlns="c84e791c-9279-4101-b0d8-1359c6bfb8a8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B86161B04886D146849F19E5CF83E5B0" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a62b97cbf4849e3933dbf3e43825b86c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="c84e791c-9279-4101-b0d8-1359c6bfb8a8" xmlns:ns3="bd192ae8-048c-430e-a712-bd4d6e23679a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd74afd4fb008876190ff6c2a71bbfd6" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -59127,72 +59184,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3569FE82-0E30-419C-9EA0-58DB8C9AA596}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bd192ae8-048c-430e-a712-bd4d6e23679a"/>
+    <ds:schemaRef ds:uri="c84e791c-9279-4101-b0d8-1359c6bfb8a8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="bd192ae8-048c-430e-a712-bd4d6e23679a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c84e791c-9279-4101-b0d8-1359c6bfb8a8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="bd192ae8-048c-430e-a712-bd4d6e23679a">
-      <UserInfo>
-        <DisplayName>Magda Bibiana Claros Rodriguez</DisplayName>
-        <AccountId>20</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Diana Patricia Murillo Quintero</DisplayName>
-        <AccountId>90</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Gerson Alejandro Saavedra Molano</DisplayName>
-        <AccountId>30</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Miguel Antonio Portilla Castro</DisplayName>
-        <AccountId>24</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan Evangelista Luna Luna</DisplayName>
-        <AccountId>36</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sandra Carolina Pena</DisplayName>
-        <AccountId>23</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Angela Daniela Naranjo Vanegas</DisplayName>
-        <AccountId>237</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>cuentadecobrocic</DisplayName>
-        <AccountId>293</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PENDIENTE xmlns="c84e791c-9279-4101-b0d8-1359c6bfb8a8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04F22BD2-2A8C-499D-9012-E6A9DE500CE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D064CE1D-2E57-49E5-9E0F-825C8EF36234}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -59210,24 +59222,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04F22BD2-2A8C-499D-9012-E6A9DE500CE6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3569FE82-0E30-419C-9EA0-58DB8C9AA596}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bd192ae8-048c-430e-a712-bd4d6e23679a"/>
-    <ds:schemaRef ds:uri="c84e791c-9279-4101-b0d8-1359c6bfb8a8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>